<commit_message>
update error compare UI
</commit_message>
<xml_diff>
--- a/logsearch/data/error_logs/UC1_UC1_新人_01.xlsx
+++ b/logsearch/data/error_logs/UC1_UC1_新人_01.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC_User\Desktop\work\logseach\ntt-backend\logsearch\data\error_logs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\demo-react\ntt-demo\ntt-backend\logsearch\data\error_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79138F6B-6B40-44EF-A5CB-77655BD4CD2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A630718E-72C6-4733-89A0-74929C59952A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="43">
   <si>
     <t>time</t>
   </si>
@@ -200,9 +200,6 @@
     <t>file:///D:/Work/AS%E7%A0%94/Git/Documents_BIST_Tsukuba2024/99_%E3%81%9D%E3%81%AE%E4%BB%96/20240415_%E6%A5%AD%E5%8B%99%E6%94%B9%E5%96%84%E3%83%87%E3%83%A2%E3%82%B7%E3%83%8A%E3%83%AA%E3%82%AA_%E8%8D%89%E6%A1%88/reserve/loginpage_reserve.html</t>
   </si>
   <si>
-    <t>UC1/UC1_ベテラン/bdot20240415_142600/0415_142656_0.png</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -298,11 +295,10 @@
     </r>
   </si>
   <si>
-    <t>UC1/UC1_ベテラン/bdot20240415_142600/0415_142722_0.png</t>
-  </si>
-  <si>
-    <t>UC1/UC1_ベテラン/bdot20240415_142600/0415_142639_0.png</t>
-    <phoneticPr fontId="6"/>
+    <t>bdot20240415_141953/0415_141958_0.png</t>
+  </si>
+  <si>
+    <t>bdot20240415_141953/0415_142001_0.png</t>
   </si>
 </sst>
 </file>
@@ -310,10 +306,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="yyyy/mm/dd\ h:mm"/>
-    <numFmt numFmtId="177" formatCode="m/d/yyyy\ h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd\ h:mm"/>
+    <numFmt numFmtId="165" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -389,17 +385,17 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -483,9 +479,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -523,7 +519,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -629,7 +625,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -771,7 +767,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -782,29 +778,29 @@
   <dimension ref="A1:AD36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.375" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.3984375" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="26" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.875" customWidth="1"/>
-    <col min="3" max="3" width="19.25" customWidth="1"/>
-    <col min="4" max="4" width="18.25" customWidth="1"/>
-    <col min="5" max="5" width="35.25" customWidth="1"/>
-    <col min="6" max="6" width="21.375" customWidth="1"/>
-    <col min="7" max="7" width="9.75" customWidth="1"/>
-    <col min="8" max="8" width="19.125" customWidth="1"/>
-    <col min="9" max="9" width="50.25" customWidth="1"/>
-    <col min="10" max="10" width="37" customWidth="1"/>
-    <col min="11" max="11" width="44.75" customWidth="1"/>
+    <col min="2" max="2" width="18.8984375" customWidth="1"/>
+    <col min="3" max="3" width="19.19921875" customWidth="1"/>
+    <col min="4" max="4" width="18.19921875" customWidth="1"/>
+    <col min="5" max="5" width="35.19921875" customWidth="1"/>
+    <col min="6" max="6" width="21.3984375" customWidth="1"/>
+    <col min="7" max="7" width="9.69921875" customWidth="1"/>
+    <col min="8" max="8" width="19.09765625" customWidth="1"/>
+    <col min="9" max="9" width="50.19921875" customWidth="1"/>
+    <col min="10" max="10" width="56.8984375" customWidth="1"/>
+    <col min="11" max="11" width="44.69921875" customWidth="1"/>
     <col min="12" max="12" width="16" customWidth="1"/>
     <col min="13" max="13" width="26" customWidth="1"/>
-    <col min="29" max="29" width="20.625" customWidth="1"/>
-    <col min="31" max="31" width="45.625" customWidth="1"/>
+    <col min="29" max="29" width="20.59765625" customWidth="1"/>
+    <col min="31" max="31" width="45.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:30">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -862,7 +858,7 @@
       <c r="AC1" s="3"/>
       <c r="AD1" s="3"/>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:30">
       <c r="A2" s="4">
         <v>45395.597152777802</v>
       </c>
@@ -888,7 +884,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:30">
       <c r="A3" s="4">
         <v>45395.597152777802</v>
       </c>
@@ -914,7 +910,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:30">
       <c r="A4" s="4">
         <v>45395.597152777802</v>
       </c>
@@ -943,7 +939,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:30">
       <c r="A5" s="4">
         <v>45395.597152777802</v>
       </c>
@@ -972,7 +968,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:30">
       <c r="A6" s="4">
         <v>45395.597199074102</v>
       </c>
@@ -1000,14 +996,14 @@
       <c r="I6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J6" t="s">
-        <v>43</v>
+      <c r="J6" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="K6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:30">
       <c r="A7" s="4">
         <v>45395.597233796303</v>
       </c>
@@ -1035,14 +1031,14 @@
       <c r="I7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K7" t="s">
         <v>35</v>
       </c>
-      <c r="K7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.4">
+    </row>
+    <row r="8" spans="1:30">
       <c r="A8" s="4">
         <v>45395.597268518497</v>
       </c>
@@ -1070,14 +1066,14 @@
       <c r="I8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J8" t="s">
-        <v>35</v>
+      <c r="J8" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="K8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30">
       <c r="A9" s="4">
         <v>45395.597268518497</v>
       </c>
@@ -1105,19 +1101,19 @@
       <c r="I9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J9" t="s">
-        <v>35</v>
+      <c r="J9" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="K9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.4">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30">
       <c r="A10" s="4">
         <v>45395.597268518497</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>14</v>
@@ -1140,20 +1136,20 @@
       <c r="I10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J10" t="s">
-        <v>35</v>
+      <c r="J10" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="K10" t="s">
+        <v>39</v>
+      </c>
+      <c r="L10" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L10" s="6" t="s">
-        <v>41</v>
-      </c>
       <c r="M10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.4">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30">
       <c r="A11" s="4">
         <v>45395.597280092603</v>
       </c>
@@ -1181,14 +1177,14 @@
       <c r="I11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J11" t="s">
-        <v>35</v>
+      <c r="J11" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="K11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30">
       <c r="A12" s="4">
         <v>45395.597280092603</v>
       </c>
@@ -1216,48 +1212,48 @@
       <c r="I12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="5" t="s">
         <v>42</v>
       </c>
       <c r="K12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="4"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:6">
       <c r="A26" s="4"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:6">
       <c r="A27" s="4"/>
       <c r="F27" s="7"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:6">
       <c r="A28" s="4"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:6">
       <c r="A29" s="4"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:6">
       <c r="A30" s="4"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:6">
       <c r="A31" s="4"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:6">
       <c r="A32" s="4"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:1">
       <c r="A33" s="4"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:1">
       <c r="A34" s="4"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:1">
       <c r="A35" s="4"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:1">
       <c r="A36" s="4"/>
     </row>
   </sheetData>

</xml_diff>